<commit_message>
Auto commit at 2025-10-19 14:56:05.98
</commit_message>
<xml_diff>
--- a/chargingdata/202501-202506.xlsx
+++ b/chargingdata/202501-202506.xlsx
@@ -616,149 +616,254 @@
   </cellStyleXfs>
   <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -766,163 +871,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1232,1217 +1232,1226 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="14.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="6" width="14.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.25" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="2" customWidth="1"/>
-    <col min="12" max="12" width="19.375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.75" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="20.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.25" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" customWidth="1"/>
+    <col min="5" max="6" width="14.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.75" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.25" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="3"/>
+      <c r="M2" s="98"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="6"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="101"/>
     </row>
     <row r="4" spans="1:17" ht="27" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="83"/>
+      <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="2">
         <v>1612407.01</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="2">
         <v>892870.64</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="2">
         <v>491758.98000000004</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="5">
         <v>49617.259999999995</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="82">
         <v>64624</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="15">
+      <c r="I5" s="83"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="6">
         <v>2716.9</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="2">
         <v>7240</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="102"/>
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="2">
         <v>479204.13</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="2">
         <v>253121.28</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="2">
         <v>148255.69</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="5">
         <v>14127.53</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="82">
         <v>19135</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="15">
+      <c r="I6" s="83"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="6">
         <v>819.09</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="8">
         <v>1600</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="102"/>
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="2">
         <v>31603.7</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="9">
         <v>15368.34</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="9">
         <v>9674.2800000000007</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="10">
         <v>991.48</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="103">
         <v>1296</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="15">
+      <c r="I7" s="79"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="6">
         <v>53.45</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="9">
         <v>150</v>
       </c>
-      <c r="N7" s="22"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26">
+      <c r="B8" s="95"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="12">
         <v>2123214.84</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="12">
         <v>1161360.26</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="12">
         <v>649688.94999999995</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="12">
         <v>64736.27</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="89">
         <v>85055</v>
       </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="30">
+      <c r="I8" s="51"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="14">
         <v>3589.44</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="15">
         <f>SUM(M5:M7)</f>
         <v>8990</v>
       </c>
-      <c r="O8" s="32"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="2">
         <v>169567.9</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="2">
         <v>102018.91</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="2">
         <v>36262.120000000003</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="5">
         <v>4273.8999999999996</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="82">
         <v>6023</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="7">
+      <c r="I9" s="83"/>
+      <c r="J9" s="2">
         <v>265.07</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="6">
         <v>200.34</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="L9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="2">
         <v>960</v>
       </c>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A10" s="35"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="77"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="2">
         <v>554390.69999999995</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="2">
         <v>331757.81</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="2">
         <v>118067.62</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="5">
         <v>13269.35</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="82">
         <v>18336</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="7">
+      <c r="I10" s="83"/>
+      <c r="J10" s="2">
         <v>315.27999999999997</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="6">
         <v>652.30999999999995</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="2">
         <v>1200</v>
       </c>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="26">
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="12">
         <v>723958.6</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="12">
         <v>433776.72</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="12">
         <v>154329.74</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="12">
         <v>17543.25</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="89">
         <v>24359</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="26">
+      <c r="I11" s="51"/>
+      <c r="J11" s="12">
         <v>580.35</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K11" s="14">
         <v>852.65</v>
       </c>
-      <c r="L11" s="31" t="s">
+      <c r="L11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="31">
+      <c r="M11" s="15">
         <f>SUM(M9:M10)</f>
         <v>2160</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41">
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="17">
         <v>2847173.44</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="17">
         <v>1595136.98</v>
       </c>
-      <c r="F12" s="41">
+      <c r="F12" s="17">
         <v>804018.69</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="17">
         <v>82279.520000000004</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="90">
         <v>109414</v>
       </c>
-      <c r="I12" s="40"/>
-      <c r="J12" s="41">
+      <c r="I12" s="59"/>
+      <c r="J12" s="17">
         <v>580.35</v>
       </c>
-      <c r="K12" s="43">
+      <c r="K12" s="18">
         <v>4442.09</v>
       </c>
-      <c r="L12" s="44" t="s">
+      <c r="L12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M12" s="44">
+      <c r="M12" s="19">
         <f>M11+M8</f>
         <v>11150</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="92"/>
+      <c r="M13" s="93"/>
     </row>
     <row r="14" spans="1:17" ht="27" x14ac:dyDescent="0.15">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="83"/>
+      <c r="D14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="7" t="s">
+      <c r="I14" s="83"/>
+      <c r="J14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L14" s="49" t="s">
+      <c r="L14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="7">
+      <c r="C15" s="86"/>
+      <c r="D15" s="2">
         <v>1800600</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="2">
         <v>968803.3</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="2">
         <v>-5301.7</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="5">
         <v>188192.99</v>
       </c>
-      <c r="H15" s="51">
+      <c r="H15" s="87">
         <v>1039.74</v>
       </c>
-      <c r="I15" s="52"/>
-      <c r="J15" s="53">
+      <c r="I15" s="88"/>
+      <c r="J15" s="22">
         <v>0.1045</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="6">
         <v>0.54</v>
       </c>
-      <c r="L15" s="54">
+      <c r="L15" s="23">
         <v>0.6</v>
       </c>
-      <c r="M15" s="53">
+      <c r="M15" s="22">
         <v>5.1299999999999998E-2</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A16" s="35"/>
-      <c r="B16" s="50" t="s">
+      <c r="A16" s="77"/>
+      <c r="B16" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="7">
+      <c r="C16" s="86"/>
+      <c r="D16" s="2">
         <v>548220</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="2">
         <v>283635.46000000002</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="2">
         <v>-1937.09</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="5">
         <v>69015.87</v>
       </c>
-      <c r="H16" s="51">
+      <c r="H16" s="87">
         <v>381.3</v>
       </c>
-      <c r="I16" s="52"/>
-      <c r="J16" s="53">
+      <c r="I16" s="88"/>
+      <c r="J16" s="22">
         <v>0.12590000000000001</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="6">
         <v>0.51</v>
       </c>
-      <c r="L16" s="54">
+      <c r="L16" s="23">
         <v>0.59</v>
       </c>
-      <c r="M16" s="53">
+      <c r="M16" s="22">
         <v>6.8900000000000003E-2</v>
       </c>
-      <c r="O16" s="55"/>
+      <c r="O16" s="24"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="26">
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="12">
         <v>2348820</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="12">
         <v>1252438.76</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="12">
         <v>-7238.79</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="12">
         <v>257208.86</v>
       </c>
-      <c r="H17" s="56">
+      <c r="H17" s="55">
         <v>1421.04</v>
       </c>
-      <c r="I17" s="57"/>
-      <c r="J17" s="58">
+      <c r="I17" s="56"/>
+      <c r="J17" s="25">
         <v>0.1095</v>
       </c>
-      <c r="K17" s="30">
+      <c r="K17" s="14">
         <v>0.53</v>
       </c>
-      <c r="L17" s="59">
+      <c r="L17" s="26">
         <v>0.6</v>
       </c>
-      <c r="M17" s="60">
+      <c r="M17" s="27">
         <v>5.4399999999999997E-2</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29">
+      <c r="C18" s="51"/>
+      <c r="D18" s="13">
         <v>802620</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="13">
         <v>463519.75</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="13">
         <v>-3222.16</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="12">
         <v>78661.399999999994</v>
       </c>
-      <c r="H18" s="56">
+      <c r="H18" s="55">
         <v>434.59</v>
       </c>
-      <c r="I18" s="57"/>
-      <c r="J18" s="58">
+      <c r="I18" s="56"/>
+      <c r="J18" s="25">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="K18" s="30">
+      <c r="K18" s="14">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L18" s="59">
+      <c r="L18" s="26">
         <v>0.64</v>
       </c>
-      <c r="M18" s="60">
+      <c r="M18" s="27">
         <v>7.7200000000000005E-2</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41">
+      <c r="B19" s="58"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="17">
         <v>3151440</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="17">
         <v>1715958.51</v>
       </c>
-      <c r="F19" s="41">
+      <c r="F19" s="17">
         <v>-10460.950000000001</v>
       </c>
-      <c r="G19" s="41">
+      <c r="G19" s="17">
         <v>335870.26</v>
       </c>
-      <c r="H19" s="62">
+      <c r="H19" s="60">
         <v>1855.64</v>
       </c>
-      <c r="I19" s="63"/>
-      <c r="J19" s="64">
+      <c r="I19" s="61"/>
+      <c r="J19" s="28">
         <v>0.1066</v>
       </c>
-      <c r="K19" s="43">
+      <c r="K19" s="18">
         <v>0.54</v>
       </c>
-      <c r="L19" s="65">
+      <c r="L19" s="29">
         <v>0.6</v>
       </c>
-      <c r="M19" s="53">
+      <c r="M19" s="22">
         <v>5.8799999999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="67"/>
-      <c r="L20" s="67"/>
-      <c r="M20" s="68"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="64"/>
     </row>
     <row r="21" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="83"/>
+      <c r="D21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="8" t="s">
+      <c r="I21" s="83"/>
+      <c r="J21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L21" s="49" t="s">
+      <c r="L21" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="M21" s="8" t="s">
+      <c r="M21" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="70">
+      <c r="C22" s="79"/>
+      <c r="D22" s="30">
         <v>2.71</v>
       </c>
-      <c r="E22" s="71">
+      <c r="E22" s="31">
         <v>0.1129</v>
       </c>
-      <c r="F22" s="70">
+      <c r="F22" s="30">
         <v>88.2</v>
       </c>
-      <c r="G22" s="70">
+      <c r="G22" s="30">
         <v>26.9</v>
       </c>
-      <c r="H22" s="72">
+      <c r="H22" s="80">
         <v>32.5</v>
       </c>
-      <c r="I22" s="73"/>
-      <c r="J22" s="70">
+      <c r="I22" s="81"/>
+      <c r="J22" s="30">
         <v>3.54</v>
       </c>
-      <c r="K22" s="70">
+      <c r="K22" s="30">
         <v>24.95</v>
       </c>
-      <c r="L22" s="74">
+      <c r="L22" s="32">
         <v>46.07</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="2">
         <v>0.86</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A23" s="35"/>
-      <c r="B23" s="69" t="s">
+      <c r="A23" s="77"/>
+      <c r="B23" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="70">
+      <c r="C23" s="79"/>
+      <c r="D23" s="30">
         <v>3.25</v>
       </c>
-      <c r="E23" s="71">
+      <c r="E23" s="31">
         <v>0.13539999999999999</v>
       </c>
-      <c r="F23" s="70">
+      <c r="F23" s="30">
         <v>115.11</v>
       </c>
-      <c r="G23" s="70">
+      <c r="G23" s="30">
         <v>35.61</v>
       </c>
-      <c r="H23" s="72">
+      <c r="H23" s="80">
         <v>33.92</v>
       </c>
-      <c r="I23" s="73"/>
-      <c r="J23" s="70">
+      <c r="I23" s="81"/>
+      <c r="J23" s="30">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K23" s="70">
+      <c r="K23" s="30">
         <v>25.04</v>
       </c>
-      <c r="L23" s="74">
+      <c r="L23" s="32">
         <v>44.3</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="2">
         <v>0.84</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="30">
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="14">
         <v>2.79</v>
       </c>
-      <c r="E24" s="58">
+      <c r="E24" s="25">
         <v>0.1163</v>
       </c>
-      <c r="F24" s="30">
+      <c r="F24" s="14">
         <v>92.37</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="14">
         <v>28.26</v>
       </c>
-      <c r="H24" s="56">
+      <c r="H24" s="55">
         <v>32.799999999999997</v>
       </c>
-      <c r="I24" s="57"/>
-      <c r="J24" s="30">
+      <c r="I24" s="56"/>
+      <c r="J24" s="14">
         <v>3.7</v>
       </c>
-      <c r="K24" s="30">
+      <c r="K24" s="14">
         <v>24.96</v>
       </c>
-      <c r="L24" s="75">
+      <c r="L24" s="33">
         <v>45.67</v>
       </c>
-      <c r="M24" s="31">
+      <c r="M24" s="15">
         <v>0.85</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="30">
+      <c r="C25" s="51"/>
+      <c r="D25" s="14">
         <v>2.69</v>
       </c>
-      <c r="E25" s="58">
+      <c r="E25" s="25">
         <v>0.11210000000000001</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="14">
         <v>111.1</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="14">
         <v>23.68</v>
       </c>
-      <c r="H25" s="56">
+      <c r="H25" s="55">
         <v>41.27</v>
       </c>
-      <c r="I25" s="57"/>
-      <c r="J25" s="30">
+      <c r="I25" s="56"/>
+      <c r="J25" s="14">
         <v>3.74</v>
       </c>
-      <c r="K25" s="30">
+      <c r="K25" s="14">
         <v>29.72</v>
       </c>
-      <c r="L25" s="75">
+      <c r="L25" s="33">
         <v>43.21</v>
       </c>
-      <c r="M25" s="31">
+      <c r="M25" s="15">
         <v>0.81</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="43">
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="18">
         <v>2.77</v>
       </c>
-      <c r="E26" s="64">
+      <c r="E26" s="28">
         <v>0.1154</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="18">
         <v>96.5</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="18">
         <v>27.25</v>
       </c>
-      <c r="H26" s="62">
+      <c r="H26" s="60">
         <v>34.6</v>
       </c>
-      <c r="I26" s="63"/>
-      <c r="J26" s="43">
+      <c r="I26" s="61"/>
+      <c r="J26" s="18">
         <v>3.71</v>
       </c>
-      <c r="K26" s="43">
+      <c r="K26" s="18">
         <v>26.02</v>
       </c>
-      <c r="L26" s="76">
+      <c r="L26" s="34">
         <v>45.12</v>
       </c>
-      <c r="M26" s="44">
+      <c r="M26" s="19">
         <v>0.84</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="68"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="64"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="79"/>
-      <c r="D28" s="80" t="s">
+      <c r="C28" s="68"/>
+      <c r="D28" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="81" t="s">
+      <c r="E28" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="82"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="82"/>
-      <c r="J28" s="83"/>
-      <c r="K28" s="81" t="s">
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="L28" s="82"/>
-      <c r="M28" s="83"/>
+      <c r="L28" s="74"/>
+      <c r="M28" s="75"/>
     </row>
     <row r="29" spans="1:13" ht="27" x14ac:dyDescent="0.15">
-      <c r="A29" s="84"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="88" t="s">
+      <c r="A29" s="66"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="88" t="s">
+      <c r="F29" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="88" t="s">
+      <c r="G29" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="H29" s="89" t="s">
+      <c r="H29" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="I29" s="88" t="s">
+      <c r="I29" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="90" t="s">
+      <c r="J29" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="K29" s="8" t="s">
+      <c r="K29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L29" s="54" t="s">
+      <c r="L29" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="M29" s="88" t="s">
+      <c r="M29" s="35" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="92" t="s">
+      <c r="B30" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="92"/>
-      <c r="D30" s="13">
+      <c r="C30" s="47"/>
+      <c r="D30" s="5">
         <v>1384629.62</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="5">
         <v>963501.6</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="10">
         <v>19603.330000000002</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="10">
         <v>8283.16</v>
       </c>
-      <c r="H30" s="18">
-        <v>1028.97</v>
-      </c>
-      <c r="I30" s="93"/>
-      <c r="J30" s="19">
+      <c r="H30" s="9">
+        <f>6192.59+204.02</f>
+        <v>6396.6100000000006</v>
+      </c>
+      <c r="I30" s="38"/>
+      <c r="J30" s="10">
         <f>IFERROR((I30+H30+G30+F30+E30),"")</f>
-        <v>992417.05999999994</v>
-      </c>
-      <c r="K30" s="7">
+        <v>997784.7</v>
+      </c>
+      <c r="K30" s="2">
         <v>0.26</v>
       </c>
-      <c r="L30" s="94">
+      <c r="L30" s="39">
         <f>IFERROR((M30/D30),"")</f>
-        <v>0.28326171442150727</v>
-      </c>
-      <c r="M30" s="95">
+        <v>0.27938512538826094</v>
+      </c>
+      <c r="M30" s="40">
         <f>IFERROR((D30-J30),"")</f>
-        <v>392212.56000000017</v>
+        <v>386844.92000000016</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A31" s="91"/>
-      <c r="B31" s="92" t="s">
+      <c r="A31" s="46"/>
+      <c r="B31" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="92"/>
-      <c r="D31" s="13">
+      <c r="C31" s="47"/>
+      <c r="D31" s="5">
         <v>401376.97</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="5">
         <v>281698.37</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="10">
         <v>5921.08</v>
       </c>
-      <c r="G31" s="19">
+      <c r="G31" s="10">
         <v>2404.83</v>
       </c>
-      <c r="H31" s="18">
-        <v>899.33</v>
-      </c>
-      <c r="I31" s="93"/>
-      <c r="J31" s="19">
+      <c r="H31" s="9">
+        <v>4330.4799999999996</v>
+      </c>
+      <c r="I31" s="38"/>
+      <c r="J31" s="10">
         <f t="shared" ref="J31:J34" si="0">IFERROR((I31+H31+G31+F31+E31),"")</f>
-        <v>290923.61</v>
-      </c>
-      <c r="K31" s="7">
+        <v>294354.76</v>
+      </c>
+      <c r="K31" s="2">
         <v>0.25</v>
       </c>
-      <c r="L31" s="94">
+      <c r="L31" s="39">
         <f t="shared" ref="L31:L35" si="1">IFERROR((M31/D31),"")</f>
-        <v>0.27518609251547244</v>
-      </c>
-      <c r="M31" s="95">
+        <v>0.266637644905237</v>
+      </c>
+      <c r="M31" s="40">
         <f t="shared" ref="M31:M34" si="2">IFERROR((D31-J31),"")</f>
-        <v>110453.35999999999</v>
+        <v>107022.20999999996</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A32" s="91"/>
-      <c r="B32" s="96" t="s">
+      <c r="A32" s="46"/>
+      <c r="B32" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="92"/>
-      <c r="D32" s="13">
+      <c r="C32" s="47"/>
+      <c r="D32" s="5">
         <v>25042.62</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="2">
         <v>15368.34</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="9">
         <v>385.03</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="10">
         <v>149.68</v>
       </c>
-      <c r="H32" s="18">
-        <v>212.12</v>
-      </c>
-      <c r="I32" s="93"/>
-      <c r="J32" s="19">
+      <c r="H32" s="9">
+        <f>3573.64+168.84</f>
+        <v>3742.48</v>
+      </c>
+      <c r="I32" s="38"/>
+      <c r="J32" s="10">
         <f t="shared" si="0"/>
-        <v>16115.17</v>
-      </c>
-      <c r="K32" s="7">
+        <v>19645.53</v>
+      </c>
+      <c r="K32" s="2">
         <v>0.25</v>
       </c>
-      <c r="L32" s="94">
+      <c r="L32" s="39">
         <f t="shared" si="1"/>
-        <v>0.35649025541257262</v>
-      </c>
-      <c r="M32" s="95">
+        <v>0.21551618800269301</v>
+      </c>
+      <c r="M32" s="40">
         <f t="shared" si="2"/>
-        <v>8927.4499999999989</v>
+        <v>5397.09</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="26">
+      <c r="B33" s="50"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="12">
         <v>1811049.21</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E33" s="12">
         <v>1260568.31</v>
       </c>
-      <c r="F33" s="26">
+      <c r="F33" s="12">
         <v>25909.439999999999</v>
       </c>
-      <c r="G33" s="26">
+      <c r="G33" s="12">
         <v>0</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="13">
         <f>H30+H31+H32</f>
-        <v>2140.42</v>
-      </c>
-      <c r="I33" s="29"/>
-      <c r="J33" s="26">
+        <v>14469.57</v>
+      </c>
+      <c r="I33" s="13"/>
+      <c r="J33" s="12">
         <f>IFERROR((I33+H33+G33+F33+E33),"")</f>
-        <v>1288618.1700000002</v>
-      </c>
-      <c r="K33" s="31">
+        <v>1300947.32</v>
+      </c>
+      <c r="K33" s="15">
         <v>0.25</v>
       </c>
-      <c r="L33" s="97">
+      <c r="L33" s="41">
         <f t="shared" si="1"/>
-        <v>0.28846871587768719</v>
-      </c>
-      <c r="M33" s="98">
+        <v>0.28166097706422893</v>
+      </c>
+      <c r="M33" s="42">
         <f t="shared" si="2"/>
-        <v>522431.0399999998</v>
+        <v>510101.8899999999</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="99" t="s">
+      <c r="B34" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="100"/>
-      <c r="D34" s="26">
+      <c r="C34" s="53"/>
+      <c r="D34" s="12">
         <v>588686.81000000006</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E34" s="12">
         <v>460297.59</v>
       </c>
-      <c r="F34" s="29">
+      <c r="F34" s="13">
         <v>0</v>
       </c>
-      <c r="G34" s="26">
+      <c r="G34" s="12">
         <v>3528.64</v>
       </c>
-      <c r="H34" s="29">
-        <v>973.02</v>
-      </c>
-      <c r="I34" s="29"/>
-      <c r="J34" s="26">
+      <c r="H34" s="13">
+        <v>2703.42</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="12">
         <f t="shared" si="0"/>
-        <v>464799.25</v>
-      </c>
-      <c r="K34" s="31">
+        <v>466529.65</v>
+      </c>
+      <c r="K34" s="15">
         <v>0.17</v>
       </c>
-      <c r="L34" s="97">
+      <c r="L34" s="41">
         <f t="shared" si="1"/>
-        <v>0.21044731747939119</v>
-      </c>
-      <c r="M34" s="98">
+        <v>0.20750789371346715</v>
+      </c>
+      <c r="M34" s="42">
         <f t="shared" si="2"/>
-        <v>123887.56000000006</v>
+        <v>122157.16000000003</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A35" s="101" t="s">
+      <c r="A35" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="101"/>
-      <c r="C35" s="101"/>
-      <c r="D35" s="41">
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="17">
         <v>2399736.02</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="17">
         <v>1720865.9</v>
       </c>
-      <c r="F35" s="41">
+      <c r="F35" s="17">
         <v>25909.439999999999</v>
       </c>
-      <c r="G35" s="41">
+      <c r="G35" s="17">
         <v>3528.64</v>
       </c>
-      <c r="H35" s="44">
+      <c r="H35" s="18">
         <f>H34+H33</f>
-        <v>3113.44</v>
-      </c>
-      <c r="I35" s="44"/>
-      <c r="J35" s="41">
+        <v>17172.989999999998</v>
+      </c>
+      <c r="I35" s="19"/>
+      <c r="J35" s="17">
         <f>IFERROR((I35+H35+G35+F35+E35),"")</f>
-        <v>1753417.42</v>
-      </c>
-      <c r="K35" s="44">
+        <v>1767476.97</v>
+      </c>
+      <c r="K35" s="19">
         <v>0.24</v>
       </c>
-      <c r="L35" s="102">
+      <c r="L35" s="43">
         <f t="shared" si="1"/>
-        <v>0.26932904061672586</v>
-      </c>
-      <c r="M35" s="103">
+        <v>0.26347025036528809</v>
+      </c>
+      <c r="M35" s="44">
         <f>IFERROR((D35-J35),"")</f>
-        <v>646318.60000000009</v>
+        <v>632259.05000000005</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:M27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="B18:C18"/>
@@ -2452,35 +2461,28 @@
     <mergeCell ref="A20:M20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>